<commit_message>
Updated ready for DDD
</commit_message>
<xml_diff>
--- a/RunningOrder.xlsx
+++ b/RunningOrder.xlsx
@@ -1,54 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\async\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{744576DC-CB85-4759-A73F-C627E844D85C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="11640"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t xml:space="preserve">Introduction </t>
-  </si>
-  <si>
-    <t>Why async</t>
-  </si>
-  <si>
-    <t>Brain Teasers</t>
-  </si>
-  <si>
-    <t>Unwrapping the syntactic sugar</t>
-  </si>
-  <si>
-    <t>How async in .Net works</t>
-  </si>
-  <si>
-    <t>Async in a Console App</t>
-  </si>
-  <si>
-    <t>Async in ASP.Net</t>
-  </si>
-  <si>
-    <t>Async in UI apps</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Deadlocks</t>
   </si>
@@ -60,12 +43,24 @@
   </si>
   <si>
     <t>Running Order</t>
+  </si>
+  <si>
+    <t>Introduction + why</t>
+  </si>
+  <si>
+    <t>Brain teasers</t>
+  </si>
+  <si>
+    <t>How async in .net works + threading</t>
+  </si>
+  <si>
+    <t>Tips</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -490,162 +485,80 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="51.81640625" customWidth="1"/>
-    <col min="3" max="3" width="42.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="3">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="3">
+        <v>12</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="3">
+        <v>32</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2">
+    </row>
+    <row r="6" spans="1:2" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="3">
+        <v>39</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="3">
+        <v>47</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="3">
+        <v>50</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="3">
-        <f>A2+C2</f>
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="3">
-        <f t="shared" ref="A4:A13" si="0">A3+C3</f>
-        <v>6</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="3">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="3">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="3">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="3">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="3">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="3">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="3">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="3">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="3">
-        <f t="shared" si="0"/>
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>